<commit_message>
updated typo in encoding
</commit_message>
<xml_diff>
--- a/hasm/Resources/Instructionset with Encoding.xlsx
+++ b/hasm/Resources/Instructionset with Encoding.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Dropbox\LT Project\Architectuur\rev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\HomebrewAssembler\hasm\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -679,7 +679,7 @@
     <t>rpkk</t>
   </si>
   <si>
-    <t>LPD DST, PAIR, IMM6</t>
+    <t>LPD DST, PAIR + IMM6</t>
   </si>
 </sst>
 </file>
@@ -1324,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added parsing for special instructions
</commit_message>
<xml_diff>
--- a/hasm/Resources/Instructionset with Encoding.xlsx
+++ b/hasm/Resources/Instructionset with Encoding.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Dropbox\LT Project\Architectuur\rev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\HomebrewAssembler\hasm\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="Full with Encoding" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="216">
   <si>
     <t>Instruction</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>SRC &lt;- IMM12</t>
+  </si>
+  <si>
+    <t>SBIS SPC, IMM12</t>
   </si>
 </sst>
 </file>
@@ -943,24 +946,6 @@
   <dxfs count="6">
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1034,13 +1019,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thick">
-          <color rgb="FFC9C9C9"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FFDBDBDB"/>
         </left>
@@ -1051,6 +1029,31 @@
           <color rgb="FFDBDBDB"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FFC9C9C9"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1066,15 +1069,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:C63" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="A1:C63" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:C63"/>
   <sortState ref="A2:C63">
     <sortCondition ref="A1:A63"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" name="Instruction" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Semantic" dataDxfId="1"/>
+    <tableColumn id="1" name="Instruction" dataDxfId="2"/>
+    <tableColumn id="2" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" name="Semantic" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1345,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,7 +2746,7 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>130</v>
+        <v>215</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>210</v>
@@ -2833,7 +2836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>